<commit_message>
added one more question to the QOC
</commit_message>
<xml_diff>
--- a/Design/MathWithSound/QOC.xlsx
+++ b/Design/MathWithSound/QOC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="21210" windowHeight="10605"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="21210" windowHeight="10605"/>
   </bookViews>
   <sheets>
     <sheet name="QOC" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Legend</t>
   </si>
@@ -97,6 +97,30 @@
   </si>
   <si>
     <t>C3: Can take a while if the QR code is broken</t>
+  </si>
+  <si>
+    <t>Q3: How do I use functions in the application?</t>
+  </si>
+  <si>
+    <t>O1: Chose the function name</t>
+  </si>
+  <si>
+    <t>C1: The functions are in a list so you can see all of the functions</t>
+  </si>
+  <si>
+    <t>C2: The function will pre-populate their correspondinig draw method</t>
+  </si>
+  <si>
+    <t>C3: You can edit the function parameters before drawing</t>
+  </si>
+  <si>
+    <t>O2: Select it from the list using the mouse</t>
+  </si>
+  <si>
+    <t>C1: Usefull if the microfone is not working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2: High precision, functions may have similar names </t>
   </si>
 </sst>
 </file>
@@ -187,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -225,6 +249,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +541,7 @@
   <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1101,11 +1126,15 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1129,11 +1158,15 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1157,11 +1190,15 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="A21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="12" t="s">
+        <v>3</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1185,11 +1222,15 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="A22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1213,11 +1254,15 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="A23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1241,11 +1286,15 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="5"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1269,11 +1318,15 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="A25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="12" t="s">
+        <v>3</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1297,11 +1350,15 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="A26" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1325,11 +1382,11 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>

</xml_diff>